<commit_message>
feature: preview support --verbose mode
</commit_message>
<xml_diff>
--- a/test/actor.xlsx
+++ b/test/actor.xlsx
@@ -2,16 +2,16 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Go XLSX"/>
-  <workbookPr showObjects="all" date1904="false"/>
+  <workbookPr showObjects="all"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" tabRatio="204" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="204" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="result" sheetId="1" r:id="rId1" state="visible"/>
   </sheets>
   <definedNames/>
-  <calcPr iterateCount="100" refMode="A1" iterateDelta="0.001"/>
+  <calcPr iterateCount="100" iterateDelta="0.001" refMode="A1"/>
 </workbook>
 </file>
 
@@ -1383,13 +1383,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <fonts count="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-      <color theme="1"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1407,16 +1407,17 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="false" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="false" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom"/>
     </xf>
   </cellXfs>
 </styleSheet>

</xml_diff>

<commit_message>
let d18n be importable by other project (#3)
* add make default .phony

* feature: preview support --verbose mode

* detect remove common.cfg

* detect package support multi goroutine callback

* lint package support multi goroutine callback

* remove package global variables

* update go.mod make d18n importable

* doc: mv logo into doc/images

Co-authored-by: zouyong007 <zouyong007@ke.com>
</commit_message>
<xml_diff>
--- a/test/actor.xlsx
+++ b/test/actor.xlsx
@@ -2,16 +2,16 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Go XLSX"/>
-  <workbookPr showObjects="all" date1904="false"/>
+  <workbookPr showObjects="all"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" tabRatio="204" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="204" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="result" sheetId="1" r:id="rId1" state="visible"/>
   </sheets>
   <definedNames/>
-  <calcPr iterateCount="100" refMode="A1" iterateDelta="0.001"/>
+  <calcPr iterateCount="100" iterateDelta="0.001" refMode="A1"/>
 </workbook>
 </file>
 
@@ -1383,13 +1383,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <fonts count="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-      <color theme="1"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1407,16 +1407,17 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="false" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="false" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom"/>
     </xf>
   </cellXfs>
 </styleSheet>

</xml_diff>